<commit_message>
made translatinator.py into an exe
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="translation" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,30 +20,228 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Original</t>
-  </si>
-  <si>
-    <t xml:space="preserve">我们偷来的这些钱可以藏在哪里？ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">我不断接到一个叫泰勒的人的电话 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">如果土拨鼠可以夹木头，土拨鼠能夹多少木头。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">في سن ال 50 ، كل شخص لديه الوجه الذي يستحقه. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demain, au lever du soleil, je ne serai plus là </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pardonnez-moi, monsieur </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No sé lo que puedo parecerle al mundo. Pero en cuanto a mí mismo, parece que he sido solo como un niño jugando en la orilla del mar y distrayéndome de vez en cuando para encontrar un guijarro más suave o una concha más bonita que la ordinaria, mientras que el gran océano de la verdad yacía sin descubrir ante mí.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+  <si>
+    <t xml:space="preserve">original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translation test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الثروة تفضل الجريء </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortune favors the bold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">arabic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wealth favors the bold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">我思故我在。 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think, therefore I am. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chinese (simplified)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cogito ergo sum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">時間就是金錢。 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time is money. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chinese (traditional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time is money.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veni vidi vici. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I came, I saw, I conquered. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">latin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I came, I saw, I won.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn das Leben dir Zitronen gibt, mach Limonade daraus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When life gives you lemons, make lemonade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">german</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When life gives you lemons, make lemonade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">अभ्यास परिपूर्ण बनाता है। </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practice makes perfect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hindi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practice Makes Perfect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tá cumhacht ag eolas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knowledge is power. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">irish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knowledge is power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non temere la perfezione, non la raggiungerai mai. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have no fear of perfection, you'll never reach it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">italian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not fear perfection, you will never reach it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千里の道も一歩から。 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The journey of a thousand miles begins with one step. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">japanese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From the journey of a thousand miles an inch.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">우리를 죽이지 않는 것은 우리를 더 강하게 만든다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">That which does not kill us makes us stronger. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">korean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What doesn't kill us makes us stronger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quand les choses se corsent, les coriaces s'y mettent. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the going gets tough, the tough get going. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">french</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the going gets tough, the tough get going.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Займитесь жизнью или займитесь смертью. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get busy living or get busy dying. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">russian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get busy with life or get busy with death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Краще любити і втратити, ніж взагалі ніколи не любити. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tis better to have loved and lost than to have never loved at all. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukranian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is better to love and lose than never to love at all.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracisz 100 procent ujęć, których nigdy nie robisz. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You miss 100 percent of the shots you never take. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">polish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You lose 100 percent of the shots you never take.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">За двадесет година од сада ћете бити више разочарани стварима које нисте урадили него онима које јесте. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twenty years from now you will be more disappointed by the things that you didn’t do than by the ones you did do. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">serbian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twenty years from now, you'll be more disappointed by the things you didn't do than the things you did.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livet är som en chokladask. Du vet aldrig vad du kommer att få. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life is like a box of chocolates. You never know what you’re going to get. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">swedish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life is like a box of chocolates. You never know what you will get.</t>
   </si>
 </sst>
 </file>
@@ -54,7 +252,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -88,22 +286,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -147,12 +345,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,15 +358,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,61 +383,260 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>